<commit_message>
New arduino files with ADC
</commit_message>
<xml_diff>
--- a/Gráficas/Linealización-In-Out(Motor)/Linealización-Motores.xlsx
+++ b/Gráficas/Linealización-In-Out(Motor)/Linealización-Motores.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alejandro.perez\Desktop\TG2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\juanm\Desktop\TG-II\GitHub\Gráficas\Linealización-In-Out(Motor)\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{753DDE67-45DD-42F0-BFC3-922C96C42A50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB670AEB-5C39-4A25-B65D-2F5D9F07BB2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{8C67850B-DC67-4CEE-82F7-75CEF2BCCA23}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{8C67850B-DC67-4CEE-82F7-75CEF2BCCA23}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
   <si>
     <t>Grados real</t>
   </si>
@@ -60,10 +60,19 @@
     <t>Diferencia</t>
   </si>
   <si>
-    <t>voltios 30-150</t>
+    <t>Diferenacia</t>
   </si>
   <si>
-    <t>diferenacia</t>
+    <t>Cuadrado</t>
+  </si>
+  <si>
+    <t>Grados Reales</t>
+  </si>
+  <si>
+    <t>Voltios Reales</t>
+  </si>
+  <si>
+    <t>Voltio Teóricos (Linealizados)</t>
   </si>
 </sst>
 </file>
@@ -99,13 +108,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -127,7 +139,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -626,7 +638,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1125,7 +1137,7 @@
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1317,11 +1329,11 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$I$1</c:f>
+              <c:f>Sheet1!$K$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>voltios 30-150</c:v>
+                  <c:v>Voltio Teóricos (Linealizados)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1352,7 +1364,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$I$2:$I$20</c:f>
+              <c:f>Sheet1!$K$2:$K$20</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="19"/>
@@ -3258,13 +3270,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>15</xdr:col>
+      <xdr:col>17</xdr:col>
       <xdr:colOff>236220</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>144780</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
+      <xdr:col>22</xdr:col>
       <xdr:colOff>426720</xdr:colOff>
       <xdr:row>15</xdr:row>
       <xdr:rowOff>83820</xdr:rowOff>
@@ -3294,16 +3306,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>350520</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>68580</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>417195</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>87630</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>228600</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>45720</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>409575</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>64770</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3330,16 +3342,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>601980</xdr:colOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>621030</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>121920</xdr:rowOff>
+      <xdr:rowOff>169545</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>342900</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
       <xdr:row>36</xdr:row>
-      <xdr:rowOff>121920</xdr:rowOff>
+      <xdr:rowOff>169545</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3368,7 +3380,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -3664,23 +3676,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2BB1C26-6301-43A6-B7C9-633B13DD8A24}">
-  <dimension ref="A1:J20"/>
+  <dimension ref="A1:M22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView tabSelected="1" topLeftCell="C34" workbookViewId="0">
+      <selection activeCell="M21" sqref="M21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.5546875" customWidth="1"/>
-    <col min="2" max="2" width="13.21875" customWidth="1"/>
-    <col min="3" max="3" width="19.109375" customWidth="1"/>
-    <col min="4" max="4" width="16.77734375" customWidth="1"/>
-    <col min="6" max="6" width="25.6640625" customWidth="1"/>
-    <col min="9" max="9" width="17.21875" customWidth="1"/>
+    <col min="1" max="1" width="17.5703125" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" customWidth="1"/>
+    <col min="3" max="3" width="19.140625" customWidth="1"/>
+    <col min="4" max="4" width="16.7109375" customWidth="1"/>
+    <col min="6" max="6" width="27.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.7109375" customWidth="1"/>
+    <col min="9" max="9" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="27.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3699,14 +3717,23 @@
       <c r="G1" t="s">
         <v>1</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="L1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="J1" t="s">
+      <c r="M1" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -3729,16 +3756,26 @@
         <f>C2-F2</f>
         <v>5.7142858000000019E-2</v>
       </c>
-      <c r="I2">
+      <c r="I2" s="3">
+        <v>0</v>
+      </c>
+      <c r="J2" s="3">
+        <v>0.52</v>
+      </c>
+      <c r="K2" s="3">
         <f>0.0144166667*A2+0.437499999</f>
         <v>0.43749999899999997</v>
       </c>
-      <c r="J2">
-        <f>C2-I2</f>
+      <c r="L2" s="3">
+        <f>C2-K2</f>
         <v>8.2500001000000045E-2</v>
       </c>
+      <c r="M2" s="3">
+        <f>+L2^2</f>
+        <v>6.8062501650000082E-3</v>
+      </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>10</v>
       </c>
@@ -3754,23 +3791,33 @@
         <v>4.2777778000000044E-2</v>
       </c>
       <c r="F3">
-        <f t="shared" ref="F3:F20" si="2">0.0143571429*A3 + 0.462857142</f>
+        <f t="shared" ref="F3:F19" si="2">0.0143571429*A3 + 0.462857142</f>
         <v>0.60642857100000003</v>
       </c>
       <c r="G3">
         <f t="shared" ref="G3:G20" si="3">C3-F3</f>
         <v>2.3571428999999977E-2</v>
       </c>
-      <c r="I3">
-        <f t="shared" ref="I3:I20" si="4">0.0144166667*A3+0.437499999</f>
+      <c r="I3" s="3">
+        <v>10</v>
+      </c>
+      <c r="J3" s="3">
+        <v>0.63</v>
+      </c>
+      <c r="K3" s="3">
+        <f>0.0144166667*A3+0.437499999</f>
         <v>0.58166666599999994</v>
       </c>
-      <c r="J3">
-        <f t="shared" ref="J3:J20" si="5">C3-I3</f>
+      <c r="L3" s="3">
+        <f>C3-K3</f>
         <v>4.8333334000000061E-2</v>
       </c>
+      <c r="M3" s="3">
+        <f t="shared" ref="M3:M20" si="4">+L3^2</f>
+        <v>2.3361111755555619E-3</v>
+      </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>20</v>
       </c>
@@ -3793,16 +3840,26 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="I4">
+      <c r="I4" s="3">
+        <v>20</v>
+      </c>
+      <c r="J4" s="3">
+        <v>0.75</v>
+      </c>
+      <c r="K4" s="3">
+        <f>0.0144166667*A4+0.437499999</f>
+        <v>0.72583333299999997</v>
+      </c>
+      <c r="L4" s="3">
+        <f>C4-K4</f>
+        <v>2.4166667000000031E-2</v>
+      </c>
+      <c r="M4" s="3">
         <f t="shared" si="4"/>
-        <v>0.72583333299999997</v>
-      </c>
-      <c r="J4">
-        <f t="shared" si="5"/>
-        <v>2.4166667000000031E-2</v>
+        <v>5.8402779388889048E-4</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>30</v>
       </c>
@@ -3825,16 +3882,26 @@
         <f t="shared" si="3"/>
         <v>-2.3571428999999977E-2</v>
       </c>
-      <c r="I5">
+      <c r="I5" s="3">
+        <v>30</v>
+      </c>
+      <c r="J5" s="3">
+        <v>0.87</v>
+      </c>
+      <c r="K5" s="3">
+        <f>0.0144166667*A5+0.437499999</f>
+        <v>0.87</v>
+      </c>
+      <c r="L5" s="3">
+        <f>C5-K5</f>
+        <v>0</v>
+      </c>
+      <c r="M5" s="3">
         <f t="shared" si="4"/>
-        <v>0.87</v>
-      </c>
-      <c r="J5">
-        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>40</v>
       </c>
@@ -3857,16 +3924,26 @@
         <f t="shared" si="3"/>
         <v>-3.7142857999999945E-2</v>
       </c>
-      <c r="I6">
+      <c r="I6" s="3">
+        <v>40</v>
+      </c>
+      <c r="J6" s="3">
+        <v>1</v>
+      </c>
+      <c r="K6" s="3">
+        <f>0.0144166667*A6+0.437499999</f>
+        <v>1.014166667</v>
+      </c>
+      <c r="L6" s="3">
+        <f>C6-K6</f>
+        <v>-1.4166667000000022E-2</v>
+      </c>
+      <c r="M6" s="3">
         <f t="shared" si="4"/>
-        <v>1.014166667</v>
-      </c>
-      <c r="J6">
-        <f t="shared" si="5"/>
-        <v>-1.4166667000000022E-2</v>
+        <v>2.0069445388888962E-4</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>50</v>
       </c>
@@ -3889,16 +3966,26 @@
         <f t="shared" si="3"/>
         <v>-6.0714286999999922E-2</v>
       </c>
-      <c r="I7">
+      <c r="I7" s="3">
+        <v>50</v>
+      </c>
+      <c r="J7" s="3">
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="K7" s="3">
+        <f>0.0144166667*A7+0.437499999</f>
+        <v>1.1583333339999999</v>
+      </c>
+      <c r="L7" s="3">
+        <f>C7-K7</f>
+        <v>-3.833333399999983E-2</v>
+      </c>
+      <c r="M7" s="3">
         <f t="shared" si="4"/>
-        <v>1.1583333339999999</v>
-      </c>
-      <c r="J7">
-        <f t="shared" si="5"/>
-        <v>-3.833333399999983E-2</v>
+        <v>1.4694444955555429E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>60</v>
       </c>
@@ -3921,16 +4008,26 @@
         <f t="shared" si="3"/>
         <v>-7.4285715999999891E-2</v>
       </c>
-      <c r="I8">
+      <c r="I8" s="3">
+        <v>60</v>
+      </c>
+      <c r="J8" s="3">
+        <v>1.25</v>
+      </c>
+      <c r="K8" s="3">
+        <f>0.0144166667*A8+0.437499999</f>
+        <v>1.3025000010000001</v>
+      </c>
+      <c r="L8" s="3">
+        <f>C8-K8</f>
+        <v>-5.2500001000000074E-2</v>
+      </c>
+      <c r="M8" s="3">
         <f t="shared" si="4"/>
-        <v>1.3025000010000001</v>
-      </c>
-      <c r="J8">
-        <f t="shared" si="5"/>
-        <v>-5.2500001000000074E-2</v>
+        <v>2.7562501050000087E-3</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>70</v>
       </c>
@@ -3953,16 +4050,26 @@
         <f t="shared" si="3"/>
         <v>-7.7857145000000072E-2</v>
       </c>
-      <c r="I9">
+      <c r="I9" s="3">
+        <v>70</v>
+      </c>
+      <c r="J9" s="3">
+        <v>1.39</v>
+      </c>
+      <c r="K9" s="3">
+        <f>0.0144166667*A9+0.437499999</f>
+        <v>1.446666668</v>
+      </c>
+      <c r="L9" s="3">
+        <f>C9-K9</f>
+        <v>-5.6666668000000087E-2</v>
+      </c>
+      <c r="M9" s="3">
         <f t="shared" si="4"/>
-        <v>1.446666668</v>
-      </c>
-      <c r="J9">
-        <f t="shared" si="5"/>
-        <v>-5.6666668000000087E-2</v>
+        <v>3.2111112622222339E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>80</v>
       </c>
@@ -3985,16 +4092,26 @@
         <f t="shared" si="3"/>
         <v>-8.1428574000000031E-2</v>
       </c>
-      <c r="I10">
+      <c r="I10" s="3">
+        <v>80</v>
+      </c>
+      <c r="J10" s="3">
+        <v>1.53</v>
+      </c>
+      <c r="K10" s="3">
+        <f>0.0144166667*A10+0.437499999</f>
+        <v>1.5908333349999999</v>
+      </c>
+      <c r="L10" s="3">
+        <f>C10-K10</f>
+        <v>-6.0833334999999877E-2</v>
+      </c>
+      <c r="M10" s="3">
         <f t="shared" si="4"/>
-        <v>1.5908333349999999</v>
-      </c>
-      <c r="J10">
-        <f t="shared" si="5"/>
-        <v>-6.0833334999999877E-2</v>
+        <v>3.7006946472222099E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>90</v>
       </c>
@@ -4017,16 +4134,26 @@
         <f t="shared" si="3"/>
         <v>-8.5000002999999991E-2</v>
       </c>
-      <c r="I11">
+      <c r="I11" s="3">
+        <v>90</v>
+      </c>
+      <c r="J11" s="3">
+        <v>1.67</v>
+      </c>
+      <c r="K11" s="3">
+        <f>0.0144166667*A11+0.437499999</f>
+        <v>1.735000002</v>
+      </c>
+      <c r="L11" s="3">
+        <f>C11-K11</f>
+        <v>-6.5000002000000112E-2</v>
+      </c>
+      <c r="M11" s="3">
         <f t="shared" si="4"/>
-        <v>1.735000002</v>
-      </c>
-      <c r="J11">
-        <f t="shared" si="5"/>
-        <v>-6.5000002000000112E-2</v>
+        <v>4.2250002600000185E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>100</v>
       </c>
@@ -4049,16 +4176,26 @@
         <f t="shared" si="3"/>
         <v>-8.857143199999995E-2</v>
       </c>
-      <c r="I12">
+      <c r="I12" s="3">
+        <v>100</v>
+      </c>
+      <c r="J12" s="3">
+        <v>1.81</v>
+      </c>
+      <c r="K12" s="3">
+        <f>0.0144166667*A12+0.437499999</f>
+        <v>1.879166669</v>
+      </c>
+      <c r="L12" s="3">
+        <f>C12-K12</f>
+        <v>-6.9166668999999903E-2</v>
+      </c>
+      <c r="M12" s="3">
         <f t="shared" si="4"/>
-        <v>1.879166669</v>
-      </c>
-      <c r="J12">
-        <f t="shared" si="5"/>
-        <v>-6.9166668999999903E-2</v>
+        <v>4.7840281005555475E-3</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>110</v>
       </c>
@@ -4081,16 +4218,26 @@
         <f t="shared" si="3"/>
         <v>-8.21428609999999E-2</v>
       </c>
-      <c r="I13">
+      <c r="I13" s="3">
+        <v>110</v>
+      </c>
+      <c r="J13" s="3">
+        <v>1.96</v>
+      </c>
+      <c r="K13" s="3">
+        <f>0.0144166667*A13+0.437499999</f>
+        <v>2.0233333359999999</v>
+      </c>
+      <c r="L13" s="3">
+        <f>C13-K13</f>
+        <v>-6.3333335999999907E-2</v>
+      </c>
+      <c r="M13" s="3">
         <f t="shared" si="4"/>
-        <v>2.0233333359999999</v>
-      </c>
-      <c r="J13">
-        <f t="shared" si="5"/>
-        <v>-6.3333335999999907E-2</v>
+        <v>4.0111114488888839E-3</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>120</v>
       </c>
@@ -4113,16 +4260,26 @@
         <f t="shared" si="3"/>
         <v>-7.5714290000000073E-2</v>
       </c>
-      <c r="I14">
+      <c r="I14" s="3">
+        <v>120</v>
+      </c>
+      <c r="J14" s="3">
+        <v>2.11</v>
+      </c>
+      <c r="K14" s="3">
+        <f>0.0144166667*A14+0.437499999</f>
+        <v>2.1675000030000002</v>
+      </c>
+      <c r="L14" s="3">
+        <f>C14-K14</f>
+        <v>-5.7500003000000355E-2</v>
+      </c>
+      <c r="M14" s="3">
         <f t="shared" si="4"/>
-        <v>2.1675000030000002</v>
-      </c>
-      <c r="J14">
-        <f t="shared" si="5"/>
-        <v>-5.7500003000000355E-2</v>
+        <v>3.30625034500005E-3</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>130</v>
       </c>
@@ -4145,16 +4302,26 @@
         <f t="shared" si="3"/>
         <v>-5.9285719000000014E-2</v>
       </c>
-      <c r="I15">
+      <c r="I15" s="3">
+        <v>130</v>
+      </c>
+      <c r="J15" s="3">
+        <v>2.27</v>
+      </c>
+      <c r="K15" s="3">
+        <f>0.0144166667*A15+0.437499999</f>
+        <v>2.3116666700000001</v>
+      </c>
+      <c r="L15" s="3">
+        <f>C15-K15</f>
+        <v>-4.1666670000000128E-2</v>
+      </c>
+      <c r="M15" s="3">
         <f t="shared" si="4"/>
-        <v>2.3116666700000001</v>
-      </c>
-      <c r="J15">
-        <f t="shared" si="5"/>
-        <v>-4.1666670000000128E-2</v>
+        <v>1.7361113888889107E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>140</v>
       </c>
@@ -4177,16 +4344,26 @@
         <f t="shared" si="3"/>
         <v>-4.2857147999999512E-2</v>
       </c>
-      <c r="I16">
+      <c r="I16" s="3">
+        <v>140</v>
+      </c>
+      <c r="J16" s="3">
+        <v>2.4300000000000002</v>
+      </c>
+      <c r="K16" s="3">
+        <f>0.0144166667*A16+0.437499999</f>
+        <v>2.4558333370000001</v>
+      </c>
+      <c r="L16" s="3">
+        <f>C16-K16</f>
+        <v>-2.5833336999999901E-2</v>
+      </c>
+      <c r="M16" s="3">
         <f t="shared" si="4"/>
-        <v>2.4558333370000001</v>
-      </c>
-      <c r="J16">
-        <f t="shared" si="5"/>
-        <v>-2.5833336999999901E-2</v>
+        <v>6.6736130055556383E-4</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>150</v>
       </c>
@@ -4209,16 +4386,26 @@
         <f t="shared" si="3"/>
         <v>-1.6428576999999667E-2</v>
       </c>
-      <c r="I17">
+      <c r="I17" s="3">
+        <v>150</v>
+      </c>
+      <c r="J17" s="3">
+        <v>2.6</v>
+      </c>
+      <c r="K17" s="3">
+        <f>0.0144166667*A17+0.437499999</f>
+        <v>2.600000004</v>
+      </c>
+      <c r="L17" s="3">
+        <f>C17-K17</f>
+        <v>-3.9999998868722741E-9</v>
+      </c>
+      <c r="M17" s="3">
         <f t="shared" si="4"/>
-        <v>2.600000004</v>
-      </c>
-      <c r="J17">
-        <f t="shared" si="5"/>
-        <v>-3.9999998868722741E-9</v>
+        <v>1.5999999094978206E-17</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>160</v>
       </c>
@@ -4241,16 +4428,26 @@
         <f t="shared" si="3"/>
         <v>-6.0000000523530161E-9</v>
       </c>
-      <c r="I18">
+      <c r="I18" s="3">
+        <v>160</v>
+      </c>
+      <c r="J18" s="3">
+        <v>2.76</v>
+      </c>
+      <c r="K18" s="3">
+        <f>0.0144166667*A18+0.437499999</f>
+        <v>2.7441666709999999</v>
+      </c>
+      <c r="L18" s="3">
+        <f>C18-K18</f>
+        <v>1.5833328999999896E-2</v>
+      </c>
+      <c r="M18" s="3">
         <f t="shared" si="4"/>
-        <v>2.7441666709999999</v>
-      </c>
-      <c r="J18">
-        <f t="shared" si="5"/>
-        <v>1.5833328999999896E-2</v>
+        <v>2.506943072222377E-4</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>170</v>
       </c>
@@ -4273,16 +4470,26 @@
         <f t="shared" si="3"/>
         <v>1.6428565000000006E-2</v>
       </c>
-      <c r="I19">
+      <c r="I19" s="3">
+        <v>170</v>
+      </c>
+      <c r="J19" s="3">
+        <v>2.92</v>
+      </c>
+      <c r="K19" s="3">
+        <f>0.0144166667*A19+0.437499999</f>
+        <v>2.8883333379999998</v>
+      </c>
+      <c r="L19" s="3">
+        <f>C19-K19</f>
+        <v>3.1666662000000123E-2</v>
+      </c>
+      <c r="M19" s="3">
         <f t="shared" si="4"/>
-        <v>2.8883333379999998</v>
-      </c>
-      <c r="J19">
-        <f t="shared" si="5"/>
-        <v>3.1666662000000123E-2</v>
+        <v>1.0027774822222518E-3</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>180</v>
       </c>
@@ -4298,20 +4505,50 @@
         <v>-9.9999959999999E-3</v>
       </c>
       <c r="F20">
-        <f t="shared" si="2"/>
+        <f>0.0143571429*A20 + 0.462857142</f>
         <v>3.0471428639999996</v>
       </c>
       <c r="G20">
         <f t="shared" si="3"/>
         <v>6.2857136000000313E-2</v>
       </c>
-      <c r="I20">
+      <c r="I20" s="3">
+        <v>180</v>
+      </c>
+      <c r="J20" s="3">
+        <v>3.11</v>
+      </c>
+      <c r="K20" s="3">
+        <f>0.0144166667*A20+0.437499999</f>
+        <v>3.0325000050000002</v>
+      </c>
+      <c r="L20" s="3">
+        <f>C20-K20</f>
+        <v>7.7499994999999711E-2</v>
+      </c>
+      <c r="M20" s="3">
         <f t="shared" si="4"/>
-        <v>3.0325000050000002</v>
-      </c>
-      <c r="J20">
-        <f t="shared" si="5"/>
-        <v>7.7499994999999711E-2</v>
+        <v>6.0062492249999804E-3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="D21">
+        <f>+SUM(D2:D20)</f>
+        <v>1.7850000380000011</v>
+      </c>
+      <c r="G21">
+        <f>+SUM(G2:G20)</f>
+        <v>-0.64500005699999874</v>
+      </c>
+      <c r="M21">
+        <f>+AVERAGE(M2:M20)</f>
+        <v>2.4765351556140427E-3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M22" s="3">
+        <f>+SQRT(M21)</f>
+        <v>4.9764798358016511E-2</v>
       </c>
     </row>
   </sheetData>
@@ -4322,22 +4559,22 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0F60CAE-89A6-4179-B2A0-016D4773C9F6}">
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14" style="1" customWidth="1"/>
-    <col min="2" max="2" width="16.33203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="16.28515625" style="1" customWidth="1"/>
     <col min="3" max="3" width="20" style="1" customWidth="1"/>
-    <col min="4" max="4" width="17.5546875" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.88671875" style="1"/>
+    <col min="4" max="4" width="17.5703125" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4351,7 +4588,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -4359,15 +4596,15 @@
         <v>0.52</v>
       </c>
       <c r="C2">
-        <f>(0.0142777778*B2)+0.53</f>
-        <v>0.53742444445600002</v>
+        <f>(0.0142777778*A2)+0.53</f>
+        <v>0.53</v>
       </c>
       <c r="D2" s="1">
         <f>B2-C2</f>
-        <v>-1.7424444455999999E-2</v>
+        <v>-1.0000000000000009E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>10</v>
       </c>
@@ -4375,15 +4612,15 @@
         <v>0.63</v>
       </c>
       <c r="C3">
-        <f t="shared" ref="C3:C20" si="0">(0.0142777778*B3)+0.53</f>
-        <v>0.53899500001400003</v>
+        <f t="shared" ref="C3:C20" si="0">(0.0142777778*A3)+0.53</f>
+        <v>0.67277777800000005</v>
       </c>
       <c r="D3" s="1">
         <f t="shared" ref="D3:D20" si="1">B3-C3</f>
-        <v>9.1004999985999979E-2</v>
+        <v>-4.2777778000000044E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>20</v>
       </c>
@@ -4392,14 +4629,14 @@
       </c>
       <c r="C4">
         <f t="shared" si="0"/>
-        <v>0.54070833335000001</v>
+        <v>0.81555555600000007</v>
       </c>
       <c r="D4" s="1">
         <f t="shared" si="1"/>
-        <v>0.20929166664999999</v>
+        <v>-6.555555600000007E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>30</v>
       </c>
@@ -4408,14 +4645,14 @@
       </c>
       <c r="C5">
         <f t="shared" si="0"/>
-        <v>0.542421666686</v>
+        <v>0.95833333399999998</v>
       </c>
       <c r="D5" s="1">
         <f t="shared" si="1"/>
-        <v>0.32757833331399999</v>
+        <v>-8.8333333999999986E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>40</v>
       </c>
@@ -4424,14 +4661,14 @@
       </c>
       <c r="C6">
         <f t="shared" si="0"/>
-        <v>0.54427777779999997</v>
+        <v>1.1011111119999999</v>
       </c>
       <c r="D6" s="1">
         <f t="shared" si="1"/>
-        <v>0.45572222220000003</v>
+        <v>-0.10111111199999989</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>50</v>
       </c>
@@ -4440,14 +4677,14 @@
       </c>
       <c r="C7">
         <f t="shared" si="0"/>
-        <v>0.54599111113600007</v>
+        <v>1.24388889</v>
       </c>
       <c r="D7" s="1">
         <f t="shared" si="1"/>
-        <v>0.57400888886400003</v>
+        <v>-0.12388888999999992</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>60</v>
       </c>
@@ -4456,14 +4693,14 @@
       </c>
       <c r="C8">
         <f t="shared" si="0"/>
-        <v>0.54784722225000004</v>
+        <v>1.3866666680000002</v>
       </c>
       <c r="D8" s="1">
         <f t="shared" si="1"/>
-        <v>0.70215277774999996</v>
+        <v>-0.13666666800000016</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>70</v>
       </c>
@@ -4472,14 +4709,14 @@
       </c>
       <c r="C9">
         <f t="shared" si="0"/>
-        <v>0.54984611114199999</v>
+        <v>1.5294444460000001</v>
       </c>
       <c r="D9" s="1">
         <f t="shared" si="1"/>
-        <v>0.84015388885799991</v>
+        <v>-0.13944444600000017</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>80</v>
       </c>
@@ -4488,14 +4725,14 @@
       </c>
       <c r="C10">
         <f t="shared" si="0"/>
-        <v>0.55184500003400005</v>
+        <v>1.672222224</v>
       </c>
       <c r="D10" s="1">
         <f t="shared" si="1"/>
-        <v>0.97815499996599997</v>
+        <v>-0.14222222399999995</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>90</v>
       </c>
@@ -4504,14 +4741,14 @@
       </c>
       <c r="C11">
         <f t="shared" si="0"/>
-        <v>0.55384388892600001</v>
+        <v>1.8150000020000001</v>
       </c>
       <c r="D11" s="1">
         <f t="shared" si="1"/>
-        <v>1.1161561110739999</v>
+        <v>-0.14500000200000018</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>100</v>
       </c>
@@ -4520,14 +4757,14 @@
       </c>
       <c r="C12">
         <f t="shared" si="0"/>
-        <v>0.55584277781800007</v>
+        <v>1.95777778</v>
       </c>
       <c r="D12" s="1">
         <f t="shared" si="1"/>
-        <v>1.2541572221820001</v>
+        <v>-0.14777777999999997</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>110</v>
       </c>
@@ -4536,14 +4773,14 @@
       </c>
       <c r="C13">
         <f t="shared" si="0"/>
-        <v>0.557984444488</v>
+        <v>2.1005555579999999</v>
       </c>
       <c r="D13" s="1">
         <f t="shared" si="1"/>
-        <v>1.402015555512</v>
+        <v>-0.14055555799999997</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>120</v>
       </c>
@@ -4552,14 +4789,14 @@
       </c>
       <c r="C14">
         <f t="shared" si="0"/>
-        <v>0.56012611115800004</v>
+        <v>2.2433333360000001</v>
       </c>
       <c r="D14" s="1">
         <f t="shared" si="1"/>
-        <v>1.5498738888419998</v>
+        <v>-0.13333333600000019</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>130</v>
       </c>
@@ -4568,14 +4805,14 @@
       </c>
       <c r="C15">
         <f t="shared" si="0"/>
-        <v>0.56241055560600006</v>
+        <v>2.3861111140000002</v>
       </c>
       <c r="D15" s="1">
         <f t="shared" si="1"/>
-        <v>1.7075894443939998</v>
+        <v>-0.11611111400000018</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>140</v>
       </c>
@@ -4584,14 +4821,14 @@
       </c>
       <c r="C16">
         <f t="shared" si="0"/>
-        <v>0.56469500005400008</v>
+        <v>2.5288888920000003</v>
       </c>
       <c r="D16" s="1">
         <f t="shared" si="1"/>
-        <v>1.8653049999460001</v>
+        <v>-9.8888892000000173E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>150</v>
       </c>
@@ -4600,14 +4837,14 @@
       </c>
       <c r="C17">
         <f t="shared" si="0"/>
-        <v>0.56712222228000009</v>
+        <v>2.6716666700000005</v>
       </c>
       <c r="D17" s="1">
         <f t="shared" si="1"/>
-        <v>2.03287777772</v>
+        <v>-7.1666670000000376E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>160</v>
       </c>
@@ -4616,14 +4853,14 @@
       </c>
       <c r="C18">
         <f t="shared" si="0"/>
-        <v>0.569406666728</v>
+        <v>2.8144444479999997</v>
       </c>
       <c r="D18" s="1">
         <f t="shared" si="1"/>
-        <v>2.190593333272</v>
+        <v>-5.4444447999999923E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>170</v>
       </c>
@@ -4632,14 +4869,14 @@
       </c>
       <c r="C19">
         <f t="shared" si="0"/>
-        <v>0.57169111117600002</v>
+        <v>2.9572222259999998</v>
       </c>
       <c r="D19" s="1">
         <f t="shared" si="1"/>
-        <v>2.348308888824</v>
+        <v>-3.7222225999999914E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>180</v>
       </c>
@@ -4648,11 +4885,17 @@
       </c>
       <c r="C20">
         <f t="shared" si="0"/>
-        <v>0.57440388895799999</v>
+        <v>3.100000004</v>
       </c>
       <c r="D20" s="1">
         <f t="shared" si="1"/>
-        <v>2.535596111042</v>
+        <v>9.9999959999999E-3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D21" s="1">
+        <f>+SUM(D2:D20)</f>
+        <v>-1.7850000380000011</v>
       </c>
     </row>
   </sheetData>
@@ -4661,15 +4904,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100ED54D2EEB357024A97D56AB9E9743501" ma:contentTypeVersion="12" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="298db8bea7824e96a779c55e3c7ee825">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="8a1a2261-f2d6-44f3-a95d-c41cda87505f" xmlns:ns4="5d4df43f-0ecb-4e47-8df8-4892f9133a80" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e2808f174ed9ac42d38284a46971c547" ns3:_="" ns4:_="">
     <xsd:import namespace="8a1a2261-f2d6-44f3-a95d-c41cda87505f"/>
@@ -4884,6 +5118,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -4893,14 +5136,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8FBF66CB-EDF7-4C3A-86A2-04A83C14D4D8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{280E2CE2-4B00-4716-BB72-ABFB12CF2266}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4915,6 +5150,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8FBF66CB-EDF7-4C3A-86A2-04A83C14D4D8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>